<commit_message>
modification des fichiers de base
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO (1).xlsx
+++ b/Modèle-audit-SEO (1).xlsx
@@ -1,36 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicopatsch/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elbachirdiallo/Documents/P4_Diallo_Mamadou/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AA54FE-C4E1-5A48-B67B-2D575EF2384F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="620" windowWidth="27860" windowHeight="17380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgajbA1sRpj4h647px0Becg4xhqcQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="79">
   <si>
     <t>Catégorie</t>
   </si>
@@ -50,14 +45,230 @@
     <t>Référence</t>
   </si>
   <si>
-    <t>(SEO ou accessiblité ?)</t>
+    <t>SEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Renseigner fr dans le champs lang </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> La langue n'est pas définie</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Le navigateur doit pouvoir identifier la langue du site </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Définir une langue du site </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> La balise Title est vide </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il faut toujours décrire pour aider les algorigues de google à bien indexer les pages du site </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bien remplr la balise Title </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le site n'aura pas titre sur les barres de recherches navigateur </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accéssibilité </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absence de balise sémentique </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absence Google analytic </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absence Search Console </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisation abusive de mot clés cachés </t>
+  </si>
+  <si>
+    <t>Fichiers css et javascript trop lourd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Images pas au bon format </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisation abusive de liens sur le footer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page 2 n'est pas nommé </t>
+  </si>
+  <si>
+    <t xml:space="preserve">accéssibilité </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absence de footer sur la page contact </t>
+  </si>
+  <si>
+    <t xml:space="preserve">la page 2ne sera pas bien indexé par les algorithme </t>
+  </si>
+  <si>
+    <t xml:space="preserve">la page 2 doit être appelé Contact </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lorsqu'on est la page contact on peut pas cliqué sur les liens </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mettre de footer sur tous les pages du site </t>
+  </si>
+  <si>
+    <t>L'attribut Alt des Balises IMG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convertir les images au Png </t>
+  </si>
+  <si>
+    <t>Mettre des balises Sémentique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réduire le fichier css </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trouver des liens qualités </t>
+  </si>
+  <si>
+    <t>Paramettrer Analytics</t>
+  </si>
+  <si>
+    <t>Paramettrer Search Console</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bien définir l'attribut Alt </t>
+  </si>
+  <si>
+    <t xml:space="preserve">l'attribut Alt facilite la lecture des mal-voyants </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bien Nommer les Pages </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bien structurer Html </t>
+  </si>
+  <si>
+    <t>Compléter la balise description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Respecter l'utilisation de mot clés </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La page Conctact pas Stylisé </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bien styliser la partie Css </t>
+  </si>
+  <si>
+    <t xml:space="preserve">on a inséré des mot clés dans l'attribut Alt </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ronan-hello.fr/series/html/balises-semantiques-html </t>
+  </si>
+  <si>
+    <t>https://www.w3.org/International/questions/qa-html-language-declarations.fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://smartkeyword.io/seo-on-page-balise-title/ </t>
+  </si>
+  <si>
+    <t>La balise meta description n'est pas compléte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">il faut bien remplir  la balise meta description pour servir de mot de clés </t>
+  </si>
+  <si>
+    <t>https://smartkeyword.io/seo-on-page-balise-meta-description/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inserer des mot cles mot clés dans la balise </t>
+  </si>
+  <si>
+    <t>https://analytics.google.com/analytics/web/#/p308543181/reports/reportinghub</t>
+  </si>
+  <si>
+    <t>https://search.google.com/search-console?resource_id=https%3A%2F%2Felbachir8495.github.io%2FP4_diallo_mamadou%2F</t>
+  </si>
+  <si>
+    <t>https://optimiz.me/choix-des-mots-cles-pour-le-referencement/</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Learn/Getting_started_with_the_web/Dealing_with_files</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Web/Media/Formats/Image_types</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Web/CSS</t>
+  </si>
+  <si>
+    <t>https://optimiz.me/attribut-alt-le-alt-image/</t>
+  </si>
+  <si>
+    <t>sans l'ID de suivi google analytic on peut  pas connaitre les visiteur du site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajouter un ID de suivi pour lier le site à votre compte analytic </t>
+  </si>
+  <si>
+    <t xml:space="preserve">il faut mettre du css dans la page Contact pour bien organiser </t>
+  </si>
+  <si>
+    <t>https://www.pierre-giraud.com/html-css-apprendre-coder-cours/lien-interne-externe-ancre/</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/1603881-apprenez-a-creer-votre-site-web-avec-html5-et-css3/1605881-structurez-votre-page</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/forum/sujet/comment-appeler-les-differentes-pages-de-mon-site-27352</t>
+  </si>
+  <si>
+    <t>lier le site avec Google search console pour suivre son évolution dans les moteurs de recherches</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eviter les méthodes de black-hate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structurer le site avec des balises sémantique </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réduire les fichiers pour permettre un chargement rapide </t>
+  </si>
+  <si>
+    <t xml:space="preserve">choisir de liens de qualité et petit nombre </t>
+  </si>
+  <si>
+    <t xml:space="preserve">on peut pas suivre le site sans Search console </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mettre dans plusieur endroits du site des mots cachés pour tromper les robots </t>
+  </si>
+  <si>
+    <t>programmer avec des balises div et span n'aide pas les robot a connaitre le contenu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">des lourds fichiers reduisent la performances du site </t>
+  </si>
+  <si>
+    <t>Mettre des formats jpg, png, jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les format utilisés svg et bmp sont lourds </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sans le css la page  n'a un  visuel adapté </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mettre trop de lien </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -85,7 +296,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -119,19 +337,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -139,6 +380,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -341,107 +585,352 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" style="1" customWidth="1"/>
     <col min="7" max="26" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:26" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:26" s="4" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E3" s="4"/>
+    <row r="3" spans="1:26" s="4" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E4" s="4"/>
+    <row r="4" spans="1:26" s="4" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E5" s="4"/>
+    <row r="5" spans="1:26" s="4" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E6" s="4"/>
+    <row r="6" spans="1:26" s="4" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E7" s="4"/>
+    <row r="7" spans="1:26" s="4" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E8" s="4"/>
+    <row r="8" spans="1:26" s="4" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E9" s="4"/>
+    <row r="9" spans="1:26" s="4" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E10" s="4"/>
+    <row r="10" spans="1:26" s="4" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E11" s="4"/>
+    <row r="11" spans="1:26" s="4" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E12" s="4"/>
+    <row r="12" spans="1:26" s="4" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E13" s="4"/>
+    <row r="13" spans="1:26" s="4" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E14" s="4"/>
+    <row r="14" spans="1:26" s="4" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E15" s="4"/>
+    <row r="15" spans="1:26" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:26" s="4" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="6"/>
+    </row>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1427,6 +1916,22 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F8" r:id="rId1" xr:uid="{13A1A476-495B-3A48-9BBD-DED61B2C94BC}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{CE5442C5-FC6B-044A-96D4-CF3F59F61E9E}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{4566F836-327D-2943-BC3B-2549AC808C7F}"/>
+    <hyperlink ref="F4" r:id="rId4" xr:uid="{CD4BB8FA-D2FD-974D-8491-5CCAEF874320}"/>
+    <hyperlink ref="F5" r:id="rId5" location="/p308543181/reports/reportinghub" xr:uid="{7A0EC9DF-8308-2E49-8DBE-1DD9E7F7DA1B}"/>
+    <hyperlink ref="F6" r:id="rId6" xr:uid="{352D7BB4-0F2D-FE40-893F-7D401000B706}"/>
+    <hyperlink ref="F7" r:id="rId7" xr:uid="{40CD79CC-9966-964F-95E3-76CB78FA092A}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{64A0F54E-984F-0247-A933-19C12E26FEEF}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{60FF3A5C-8775-B14F-8FC9-A51630C32779}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{EA8D3FC8-5E75-A847-A7C2-C52BE885CFBD}"/>
+    <hyperlink ref="F15" r:id="rId11" xr:uid="{9BFF7ADF-0D69-B14A-9DCC-6F18769FB60A}"/>
+    <hyperlink ref="F12" r:id="rId12" xr:uid="{912BC8F3-5EA6-CB49-975F-AFEAD3CE856F}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{8D8D0655-7CFC-624B-9CF9-CE206A12EAFB}"/>
+    <hyperlink ref="F13" r:id="rId14" xr:uid="{0478DBEC-6546-6141-A023-8173892EA9A9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>